<commit_message>
Fix email monitoring to process all emails sequentially - stops polling while processing then checks again after completion
</commit_message>
<xml_diff>
--- a/Examples Contracts.xlsx
+++ b/Examples Contracts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Claude Code Projects\SmthosExp\arkansas-contract-agent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B5FB4B4-2323-4064-8679-0444627CAEBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01D08A4-68B6-4F9E-ADD9-905427AED7ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31200" yWindow="2850" windowWidth="28800" windowHeight="15345" xr2:uid="{AB81FE26-5223-4778-AB30-553A49DDB35E}"/>
+    <workbookView xWindow="-36930" yWindow="630" windowWidth="28800" windowHeight="15345" xr2:uid="{AB81FE26-5223-4778-AB30-553A49DDB35E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="76">
   <si>
     <t>15 Dunbarton</t>
   </si>
@@ -242,9 +242,6 @@
     <t xml:space="preserve">Termite </t>
   </si>
   <si>
-    <t>npm i -g @anthropic-ai/claude-code</t>
-  </si>
-  <si>
     <t>Buyer Agency</t>
   </si>
   <si>
@@ -257,13 +254,16 @@
     <t>Y-Seller</t>
   </si>
   <si>
-    <t>Referigerato</t>
-  </si>
-  <si>
     <t>Yes -Escapr</t>
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Y-Buyer</t>
+  </si>
+  <si>
+    <t>Referigerator</t>
   </si>
 </sst>
 </file>
@@ -680,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5BAE6E-D0A1-4B11-8A39-39BE0FE5F54D}">
-  <dimension ref="A1:Z11"/>
+  <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="T16" sqref="T16"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="X9" sqref="X9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,7 +691,6 @@
     <col min="1" max="1" width="22.5703125" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" style="11" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="11" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" customWidth="1"/>
     <col min="6" max="7" width="28.5703125" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
@@ -702,12 +701,12 @@
     <col min="20" max="20" width="12.7109375" customWidth="1"/>
     <col min="21" max="21" width="23.5703125" customWidth="1"/>
     <col min="22" max="22" width="14.7109375" customWidth="1"/>
-    <col min="23" max="23" width="19.85546875" customWidth="1"/>
-    <col min="24" max="24" width="29.42578125" customWidth="1"/>
-    <col min="26" max="26" width="56.85546875" customWidth="1"/>
+    <col min="23" max="23" width="12.85546875" customWidth="1"/>
+    <col min="24" max="24" width="6.7109375" style="11" customWidth="1"/>
+    <col min="25" max="25" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -717,9 +716,6 @@
       <c r="C1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>69</v>
-      </c>
       <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
@@ -777,11 +773,14 @@
       <c r="W1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -791,7 +790,6 @@
       <c r="C2" s="9">
         <v>2.5</v>
       </c>
-      <c r="D2" s="9"/>
       <c r="E2">
         <v>350000</v>
       </c>
@@ -846,11 +844,9 @@
       <c r="W2" t="s">
         <v>43</v>
       </c>
-      <c r="Z2" t="s">
-        <v>68</v>
-      </c>
+      <c r="X2" s="9"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -860,7 +856,6 @@
       <c r="C3" s="9">
         <v>3</v>
       </c>
-      <c r="D3" s="9"/>
       <c r="E3">
         <v>450000</v>
       </c>
@@ -915,8 +910,9 @@
       <c r="W3" t="s">
         <v>44</v>
       </c>
+      <c r="X3" s="9"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -926,7 +922,6 @@
       <c r="C4" s="9">
         <v>2.7</v>
       </c>
-      <c r="D4" s="9"/>
       <c r="E4">
         <v>600000</v>
       </c>
@@ -981,8 +976,9 @@
       <c r="W4" t="s">
         <v>44</v>
       </c>
+      <c r="X4" s="9"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -992,9 +988,6 @@
       <c r="C5" s="9">
         <v>2.7</v>
       </c>
-      <c r="D5" s="9">
-        <v>3</v>
-      </c>
       <c r="E5">
         <v>600000</v>
       </c>
@@ -1049,8 +1042,11 @@
       <c r="W5" t="s">
         <v>44</v>
       </c>
+      <c r="X5" s="9">
+        <v>3</v>
+      </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1060,7 +1056,6 @@
       <c r="C6" s="9">
         <v>2.7</v>
       </c>
-      <c r="D6" s="9"/>
       <c r="E6">
         <v>400000</v>
       </c>
@@ -1115,11 +1110,12 @@
       <c r="W6" t="s">
         <v>44</v>
       </c>
-      <c r="X6" t="s">
+      <c r="X6" s="9"/>
+      <c r="Y6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
@@ -1129,7 +1125,6 @@
       <c r="C7" s="10">
         <v>2.7</v>
       </c>
-      <c r="D7" s="10"/>
       <c r="E7" s="5">
         <v>500000</v>
       </c>
@@ -1187,8 +1182,9 @@
       <c r="W7" t="s">
         <v>44</v>
       </c>
+      <c r="X7" s="10"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1198,15 +1194,14 @@
       <c r="C8" s="9">
         <v>2.7</v>
       </c>
-      <c r="D8" s="9"/>
       <c r="E8">
         <v>250000</v>
       </c>
       <c r="F8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" t="s">
         <v>70</v>
-      </c>
-      <c r="G8" t="s">
-        <v>71</v>
       </c>
       <c r="H8" t="s">
         <v>50</v>
@@ -1224,19 +1219,19 @@
         <v>22</v>
       </c>
       <c r="M8" t="s">
+        <v>71</v>
+      </c>
+      <c r="N8" t="s">
+        <v>75</v>
+      </c>
+      <c r="O8" t="s">
         <v>72</v>
       </c>
-      <c r="N8" t="s">
+      <c r="P8" t="s">
         <v>73</v>
       </c>
-      <c r="O8" t="s">
-        <v>74</v>
-      </c>
-      <c r="P8" t="s">
-        <v>75</v>
-      </c>
       <c r="Q8" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="R8" s="3">
         <v>45989</v>
@@ -1256,8 +1251,11 @@
       <c r="W8" t="s">
         <v>44</v>
       </c>
+      <c r="X8" s="9">
+        <v>2</v>
+      </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1267,9 +1265,65 @@
       <c r="C9" s="9">
         <v>3</v>
       </c>
-      <c r="D9" s="9"/>
+      <c r="E9">
+        <v>400000</v>
+      </c>
+      <c r="F9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9" t="s">
+        <v>47</v>
+      </c>
+      <c r="K9" t="s">
+        <v>47</v>
+      </c>
+      <c r="L9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M9" t="s">
+        <v>74</v>
+      </c>
+      <c r="N9" t="s">
+        <v>75</v>
+      </c>
+      <c r="O9" t="s">
+        <v>60</v>
+      </c>
+      <c r="P9" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>47</v>
+      </c>
+      <c r="R9" s="3">
+        <v>45989</v>
+      </c>
+      <c r="S9">
+        <v>2</v>
+      </c>
+      <c r="T9" s="3">
+        <v>45900</v>
+      </c>
+      <c r="U9" t="s">
+        <v>41</v>
+      </c>
+      <c r="V9" t="s">
+        <v>42</v>
+      </c>
+      <c r="W9" t="s">
+        <v>44</v>
+      </c>
+      <c r="X9" s="9">
+        <v>2</v>
+      </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1279,9 +1333,9 @@
       <c r="C10" s="9">
         <v>3</v>
       </c>
-      <c r="D10" s="9"/>
+      <c r="X10" s="9"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1291,7 +1345,7 @@
       <c r="C11" s="9">
         <v>2.7</v>
       </c>
-      <c r="D11" s="9"/>
+      <c r="X11" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Remove header and footer from agent info sheet, compress layout to fit on one page
</commit_message>
<xml_diff>
--- a/Examples Contracts.xlsx
+++ b/Examples Contracts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Claude Code Projects\SmthosExp\arkansas-contract-agent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01D08A4-68B6-4F9E-ADD9-905427AED7ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96B3152-F5FE-4575-93D6-492810136FE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36930" yWindow="630" windowWidth="28800" windowHeight="15345" xr2:uid="{AB81FE26-5223-4778-AB30-553A49DDB35E}"/>
+    <workbookView xWindow="-38520" yWindow="-45" windowWidth="38640" windowHeight="21120" xr2:uid="{AB81FE26-5223-4778-AB30-553A49DDB35E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -273,7 +273,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,6 +300,32 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF7030A0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -321,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -346,6 +372,28 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -682,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5BAE6E-D0A1-4B11-8A39-39BE0FE5F54D}">
   <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="X9" sqref="X9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -846,71 +894,71 @@
       </c>
       <c r="X2" s="9"/>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:25" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="13">
         <v>4702</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="14">
         <v>3</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="15">
         <v>450000</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="15">
         <v>5000</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P3" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="Q3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="R3" s="3">
+      <c r="R3" s="16">
         <v>45959</v>
       </c>
-      <c r="S3">
+      <c r="S3" s="15">
         <v>3.5</v>
       </c>
-      <c r="T3" s="3">
+      <c r="T3" s="16">
         <v>13026</v>
       </c>
-      <c r="U3" t="s">
+      <c r="U3" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="V3" t="s">
+      <c r="V3" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="W3" t="s">
+      <c r="W3" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="X3" s="9"/>
+      <c r="X3" s="14"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1255,71 +1303,71 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:25" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="18">
         <v>2978</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="19">
         <v>3</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="20">
         <v>400000</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="20">
         <v>0</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N9" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="O9" t="s">
+      <c r="O9" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="P9" t="s">
+      <c r="P9" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="Q9" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="R9" s="3">
+      <c r="R9" s="21">
         <v>45989</v>
       </c>
-      <c r="S9">
+      <c r="S9" s="20">
         <v>2</v>
       </c>
-      <c r="T9" s="3">
+      <c r="T9" s="21">
         <v>45900</v>
       </c>
-      <c r="U9" t="s">
+      <c r="U9" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="V9" t="s">
+      <c r="V9" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="W9" t="s">
+      <c r="W9" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="X9" s="9">
+      <c r="X9" s="19">
         <v>2</v>
       </c>
     </row>

</xml_diff>